<commit_message>
Ajuste PPT e planilha de riscos
</commit_message>
<xml_diff>
--- a/documents/xlsx/planilha_de_riscos.xlsx
+++ b/documents/xlsx/planilha_de_riscos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kakar\Desktop\BandTec\Primeiro semestre\Iniciativa 0\startech\documents\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WINDOWS10\Desktop\BandTec\noIgnite\documents\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8443684-A0F6-4FA7-8DF6-60235A00851E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1320" windowWidth="18195" windowHeight="8520"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -44,9 +45,6 @@
     <t>Perder o backup do projeto</t>
   </si>
   <si>
-    <t>Incompatibilidade de sistemas que fazem o projeto funcionar</t>
-  </si>
-  <si>
     <t>Um integrante não pode comparecer na apresentação</t>
   </si>
   <si>
@@ -130,12 +128,15 @@
   </si>
   <si>
     <t>O integrante deverá comunicar o grupo para que tanto ele quanto o grupo se adeque a nova situação.</t>
+  </si>
+  <si>
+    <t>Incompatibilidade de sistemas que fazem o projeto não funcionar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -276,11 +277,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -375,6 +376,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -410,6 +428,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -585,17 +620,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="70.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -612,38 +647,38 @@
     </row>
     <row r="3" spans="3:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
-      <c r="D3" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
+      <c r="D3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="3:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="12" t="s">
-        <v>12</v>
-      </c>
       <c r="J4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -652,7 +687,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="6">
         <v>2</v>
@@ -664,10 +699,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -676,7 +711,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="5">
         <v>1</v>
@@ -688,10 +723,10 @@
         <v>2</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="3:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -700,22 +735,22 @@
         <v>3</v>
       </c>
       <c r="E7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6">
+        <v>3</v>
+      </c>
+      <c r="H7" s="6">
+        <v>3</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="13" t="s">
         <v>20</v>
-      </c>
-      <c r="F7" s="6">
-        <v>1</v>
-      </c>
-      <c r="G7" s="6">
-        <v>3</v>
-      </c>
-      <c r="H7" s="6">
-        <v>3</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>21</v>
       </c>
       <c r="L7" s="1"/>
     </row>
@@ -725,7 +760,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="5">
         <v>2</v>
@@ -737,10 +772,10 @@
         <v>4</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>35</v>
+        <v>13</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -761,10 +796,10 @@
         <v>1</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -785,10 +820,10 @@
         <v>3</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>23</v>
+        <v>12</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -809,10 +844,10 @@
         <v>6</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -821,7 +856,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
@@ -833,10 +868,10 @@
         <v>3</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>24</v>
+        <v>12</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="3:12" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -845,7 +880,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="6">
         <v>1</v>
@@ -857,10 +892,10 @@
         <v>3</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -881,10 +916,10 @@
         <v>3</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -905,10 +940,10 @@
         <v>2</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -929,10 +964,10 @@
         <v>1</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J16" s="15" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="3:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -941,7 +976,7 @@
         <v>13</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="F17" s="6">
         <v>1</v>
@@ -953,10 +988,10 @@
         <v>1</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="3:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -965,7 +1000,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" s="7">
         <v>2</v>
@@ -977,10 +1012,10 @@
         <v>6</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>30</v>
+        <v>13</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.25">
@@ -996,7 +1031,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1008,7 +1043,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>